<commit_message>
Built site for AlpsNMR: 2.5.9002@
</commit_message>
<xml_diff>
--- a/reference/metadata.xlsx
+++ b/reference/metadata.xlsx
@@ -427,7 +427,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>/Users/runner/runners/2.262.1/work/_temp/Library/AlpsNMR/dataset-demo/10.zip</t>
+          <t>/Users/runner/runners/2.263.0/work/_temp/Library/AlpsNMR/dataset-demo/10.zip</t>
         </is>
       </c>
       <c r="E2">
@@ -465,7 +465,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>/Users/runner/runners/2.262.1/work/_temp/Library/AlpsNMR/dataset-demo/20.zip</t>
+          <t>/Users/runner/runners/2.263.0/work/_temp/Library/AlpsNMR/dataset-demo/20.zip</t>
         </is>
       </c>
       <c r="E3">
@@ -503,7 +503,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>/Users/runner/runners/2.262.1/work/_temp/Library/AlpsNMR/dataset-demo/30.zip</t>
+          <t>/Users/runner/runners/2.263.0/work/_temp/Library/AlpsNMR/dataset-demo/30.zip</t>
         </is>
       </c>
       <c r="E4">
@@ -541,7 +541,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>/Users/runner/runners/2.262.1/work/_temp/Library/AlpsNMR/dataset-demo/40.zip</t>
+          <t>/Users/runner/runners/2.263.0/work/_temp/Library/AlpsNMR/dataset-demo/40.zip</t>
         </is>
       </c>
       <c r="E5">

</xml_diff>